<commit_message>
minor fixes - runs to completion
</commit_message>
<xml_diff>
--- a/short_term_model.xlsx
+++ b/short_term_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/eam/ICIP2023-EAM-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5882153A-F836-6F4D-A0A4-E63E13193CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986E3522-6161-254F-9797-365286A83D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="10580" windowWidth="42240" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4600" yWindow="4040" windowWidth="33800" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="metadata" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>variable</t>
   </si>
@@ -242,6 +241,21 @@
   </si>
   <si>
     <t>https://openconnect.netflix.com/en_gb/appliances/</t>
+  </si>
+  <si>
+    <t>user name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ui variable</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>override</t>
   </si>
 </sst>
 </file>
@@ -252,7 +266,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -343,8 +357,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,8 +386,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF548235"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -410,11 +437,10 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -467,6 +493,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -851,21 +886,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="19" max="19" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -917,126 +952,138 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="R1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="C2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <v>7.5000000000000002E-4</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="20">
         <v>-0.2</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <v>0.1</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <v>0.05</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="21">
         <v>43831</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="16" t="s">
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <v>7.5000000000000002E-4</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>-0.2</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="20">
         <v>0.1</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <v>0.05</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="21">
         <v>43831</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="R5" s="7"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="C5" s="3"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <v>0.1</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <v>0</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>0.1</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <v>0.05</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="21">
         <v>43831</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="Q6" t="s">
@@ -1046,52 +1093,55 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="16">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="15">
         <v>1.5</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>-0.2</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <v>0.1</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="20">
         <v>0.05</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="21">
         <v>43831</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>59</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <v>0.02</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <v>-0.2</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <v>0.1</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="20">
         <v>0.05</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="21">
         <v>43831</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="Q8" t="s">
@@ -1101,97 +1151,99 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>15</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>-0.2</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <v>0.1</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <v>0.05</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="21">
         <v>43831</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18">
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17">
         <v>0.01</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="22">
         <v>0</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>0.1</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <v>0.05</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="21">
         <v>42005</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="24" t="s">
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C11" s="3"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <v>0.3</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>0</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="20">
         <v>0.1</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="20">
         <v>0.05</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="21">
         <v>43831</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="Q12" t="s">
@@ -1201,12 +1253,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="F13" s="16"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="22"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="F13" s="15"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
       <c r="Q13" t="s">
         <v>29</v>
       </c>
@@ -1214,66 +1266,66 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:20" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:22" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>0</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="20">
         <v>0.1</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="20">
         <v>0.05</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="21">
         <v>43862</v>
       </c>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:20" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="20">
         <v>0</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="20">
         <v>0.1</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="20">
         <v>0.05</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="21">
         <v>43862</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1281,28 +1333,28 @@
       <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>0</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="20">
         <v>0.1</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="20">
         <v>0.05</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="21">
         <v>43862</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="14" t="s">
         <v>53</v>
       </c>
       <c r="Q17" t="s">
@@ -1316,19 +1368,19 @@
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <v>2</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="20">
         <v>0</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="20">
         <v>0.1</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="20">
         <v>0.05</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="21">
         <v>43862</v>
       </c>
       <c r="K18" t="s">
@@ -1342,19 +1394,19 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="15">
         <v>1</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="20">
         <v>0</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="20">
         <v>0.1</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="20">
         <v>0.05</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="21">
         <v>43862</v>
       </c>
       <c r="K19" t="s">
@@ -1362,7 +1414,7 @@
       </c>
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M34" s="11"/>
+      <c r="M34" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1385,40 +1437,40 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D7" s="13"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="12"/>
+      <c r="J7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F8">
@@ -1427,10 +1479,10 @@
       <c r="G8">
         <v>0.30437500000000001</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K8">
@@ -1441,10 +1493,10 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F9">
@@ -1453,10 +1505,10 @@
       <c r="G9">
         <v>30.4375</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K9">
@@ -1467,10 +1519,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F10">
@@ -1479,10 +1531,10 @@
       <c r="G10">
         <v>6.0874999999999999E-2</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K10">
@@ -1493,10 +1545,10 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F11">
@@ -1505,10 +1557,10 @@
       <c r="G11">
         <v>22.234593749999998</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K11">
@@ -1519,10 +1571,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F12">
@@ -1531,10 +1583,10 @@
       <c r="G12">
         <v>6.0875000000000004</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K12">
@@ -1545,43 +1597,43 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="13">
         <v>0.91312499999999996</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="13">
         <v>3.6524999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E16" s="9"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="E19" s="8"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="E20" s="8"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="J21" s="9"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="J22" s="9"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1598,10 +1650,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="12">
+      <c r="B1" s="11">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new result figures near final parameters
</commit_message>
<xml_diff>
--- a/short_term_model.xlsx
+++ b/short_term_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/eam/ICIP2023-EAM-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A9988C-4E3F-5D42-81C8-FAE66A6591AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBFCF94-D1F8-AE4C-9782-7B9D5913A6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>variable</t>
   </si>
@@ -226,9 +226,6 @@
     <t>s720</t>
   </si>
   <si>
-    <t>https://www.howtogeek.com/338983/how-much-data-does-netflix-use/</t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
   </si>
   <si>
     <t>The power consumption of mobile and fixed network data services - The case of streaming video and downloading large files</t>
-  </si>
-  <si>
-    <t>https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/</t>
   </si>
   <si>
     <t>minute</t>
@@ -261,17 +255,98 @@
   </si>
   <si>
     <t>J/megabit</t>
+  </si>
+  <si>
+    <t>https://www.ofcom.org.uk/__data/assets/pdf_file/0016/242701/media-nations-report-2022.pdf</t>
+  </si>
+  <si>
+    <t>Own</t>
+  </si>
+  <si>
+    <t>laptop share</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comscore’s The US Total Video
+Report (Comscore, 2014)</t>
+  </si>
+  <si>
+    <t>S/B VoD daily audience</t>
+  </si>
+  <si>
+    <t>50.7m daily average viewers according to BARB. 12% of which on laptops according to Comscore. [https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/] [ Comscore’s The US Total Video
+Report (Comscore, 2014)]</t>
+  </si>
+  <si>
+    <t>Informed guess</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>daily viewing time</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>carbon</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Origin Datacentre</t>
+  </si>
+  <si>
+    <t>Content Delivery Network</t>
+  </si>
+  <si>
+    <t>Core Network</t>
+  </si>
+  <si>
+    <t>Access Network</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>data vol</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>Mb</t>
+  </si>
+  <si>
+    <t>energy acc</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +446,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -448,12 +535,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -519,7 +607,6 @@
     <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -529,21 +616,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -923,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -934,6 +1031,7 @@
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="59.5" hidden="1" customWidth="1"/>
     <col min="20" max="22" width="0" hidden="1" customWidth="1"/>
@@ -1030,7 +1128,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="32"/>
+      <c r="N3" s="31"/>
       <c r="Q3" s="6" t="s">
         <v>49</v>
       </c>
@@ -1038,38 +1136,38 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32">
         <v>30</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="33">
         <v>-0.2</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="33">
         <v>0.1</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="33">
         <v>0.05</v>
       </c>
-      <c r="J4" s="35">
-        <v>43831</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="33"/>
+      <c r="J4" s="34">
+        <v>44562</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="32"/>
       <c r="Q4" s="23" t="s">
         <v>52</v>
       </c>
@@ -1090,36 +1188,36 @@
       <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33">
+      <c r="E6" s="32"/>
+      <c r="F6" s="32">
         <v>0.03</v>
       </c>
-      <c r="G6" s="33">
-        <v>0</v>
-      </c>
-      <c r="H6" s="33">
+      <c r="G6" s="32">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
         <v>0.1</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="33">
         <v>0.05</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="34">
         <v>43831</v>
       </c>
-      <c r="K6" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" s="33"/>
-      <c r="M6" s="36" t="s">
-        <v>67</v>
+      <c r="K6" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="32"/>
+      <c r="M6" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="Q6" t="s">
         <v>22</v>
@@ -1129,51 +1227,51 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="36"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" spans="1:22" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33">
+      <c r="E8" s="32"/>
+      <c r="F8" s="32">
         <v>0.02</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="32">
         <v>-0.2</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="32">
         <v>0.1</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="33">
         <v>0.05</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="34">
         <v>43831</v>
       </c>
-      <c r="K8" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="L8" s="33"/>
-      <c r="M8" s="36" t="s">
-        <v>67</v>
+      <c r="K8" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="32"/>
+      <c r="M8" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -1192,7 +1290,7 @@
       <c r="K9" s="4"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>50</v>
       </c>
@@ -1201,7 +1299,7 @@
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="G10" s="21">
         <v>0</v>
@@ -1218,7 +1316,7 @@
       <c r="K10" s="17"/>
       <c r="L10" s="18"/>
       <c r="M10" s="5" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="18"/>
@@ -1240,7 +1338,7 @@
     </row>
     <row r="12" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
@@ -1263,8 +1361,8 @@
       <c r="K12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="30" t="s">
-        <v>65</v>
+      <c r="M12" s="29" t="s">
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
         <v>26</v>
@@ -1288,78 +1386,53 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E14" s="13"/>
-      <c r="F14" s="29"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:22" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="28">
         <v>50700000</v>
       </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-      <c r="H15" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="J15" s="20">
-        <v>43862</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="M15" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="M15" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="15">
-        <v>43</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-      <c r="H16" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="I16" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="J16" s="20">
-        <v>43862</v>
-      </c>
-      <c r="K16" s="13" t="s">
+      <c r="F16" s="37">
+        <v>0.12</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="M16" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="M16" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>42</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="28">
-        <v>10000000</v>
+      <c r="F17" s="38">
+        <f>F15*F16</f>
+        <v>6084000</v>
       </c>
       <c r="G17" s="19">
         <v>0</v>
@@ -1373,28 +1446,21 @@
       <c r="J17" s="20">
         <v>43862</v>
       </c>
-      <c r="K17" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>61</v>
+      <c r="K17" s="4"/>
+      <c r="M17" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="28">
-        <v>6500000</v>
+      <c r="E18" s="13"/>
+      <c r="F18" s="15">
+        <v>43</v>
       </c>
       <c r="G18" s="19">
         <v>0</v>
@@ -1406,20 +1472,24 @@
         <v>0.05</v>
       </c>
       <c r="J18" s="20">
-        <v>43862</v>
-      </c>
-      <c r="K18" s="13"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>44228</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="F19">
-        <v>6.6023598758794488</v>
+      <c r="F19" s="28">
+        <v>1688000</v>
       </c>
       <c r="G19" s="19">
         <v>0</v>
@@ -1431,18 +1501,21 @@
         <v>0.05</v>
       </c>
       <c r="J19" s="20">
-        <v>43862</v>
-      </c>
-      <c r="K19" t="s">
-        <v>45</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>60</v>
+        <v>44593</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>61</v>
@@ -1450,8 +1523,8 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="F20">
-        <v>4.7998260991263555</v>
+      <c r="F20" s="28">
+        <v>911000</v>
       </c>
       <c r="G20" s="19">
         <v>0</v>
@@ -1463,34 +1536,236 @@
         <v>0.05</v>
       </c>
       <c r="J20" s="20">
+        <v>44593</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <v>6.6023598758794488</v>
+      </c>
+      <c r="G21" s="19">
+        <v>0</v>
+      </c>
+      <c r="H21" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="J21" s="20">
         <v>43862</v>
       </c>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F21" s="14"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
-      <c r="M21" s="5"/>
+      <c r="K21" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22">
+        <v>4.7998260991263555</v>
+      </c>
+      <c r="G22" s="19">
+        <v>0</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I22" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="J22" s="20">
+        <v>43862</v>
+      </c>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F23" s="14"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="13"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L26" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E27" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="39">
+        <f>F17*F18*60</f>
+        <v>15696720000</v>
+      </c>
+      <c r="G27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="K27">
+        <v>469.40175416605479</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E28" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="39">
+        <f>F27*365/12</f>
+        <v>477441900000</v>
+      </c>
+      <c r="G28" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28">
+        <v>9857.4368374871538</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>1080</v>
+      </c>
+      <c r="J29" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29">
+        <v>6720.6160710000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="39">
+        <f>F28*F21</f>
+        <v>3152243243623.6484</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J30" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30">
+        <v>4316.8420481675757</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E31" s="13"/>
+      <c r="F31" s="39">
+        <f>F30/3600000</f>
+        <v>875623.12322879129</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J31" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31">
+        <v>876222.86509401642</v>
+      </c>
+      <c r="L31" s="39">
+        <f>K31/F31</f>
+        <v>1.0006849315068493</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="39">
+        <f>F31*F12</f>
+        <v>344995.51055214379</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E34" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="39">
+        <f>F19*F28</f>
+        <v>8.059219272E+17</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F35" s="39">
+        <f>F34/1000000</f>
+        <v>805921927200</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E36" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="39">
+        <f>F35*F8</f>
+        <v>16118438544</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F37" s="39">
+        <f>F36/3600000</f>
+        <v>4477.3440399999999</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Q10" r:id="rId1" xr:uid="{9457789D-A2B4-684F-8723-371AC82363FD}"/>
     <hyperlink ref="Q4" r:id="rId2" xr:uid="{770F17AD-6F52-D749-93D4-3560E5A28FFE}"/>
-    <hyperlink ref="M17" r:id="rId3" xr:uid="{796A6ADE-9F8F-6540-AEC1-DD8EEAE3466A}"/>
-    <hyperlink ref="M12" r:id="rId4" display="https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf" xr:uid="{F9266DB3-7397-8F48-83F2-55D825A1A6CA}"/>
-    <hyperlink ref="M16" r:id="rId5" xr:uid="{13F557E0-5A18-8140-A2C7-150350381894}"/>
-    <hyperlink ref="M15" r:id="rId6" display="https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/_x000a__x000a_Ofcom finds the viewing time has remained largely similar since pandemic ()" xr:uid="{78A7B747-76E0-D749-A511-4A5793808055}"/>
+    <hyperlink ref="M12" r:id="rId3" display="https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf" xr:uid="{F9266DB3-7397-8F48-83F2-55D825A1A6CA}"/>
+    <hyperlink ref="M18" r:id="rId4" xr:uid="{13F557E0-5A18-8140-A2C7-150350381894}"/>
+    <hyperlink ref="M15" r:id="rId5" display="https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/_x000a__x000a_Ofcom finds the viewing time has remained largely similar since pandemic ()" xr:uid="{78A7B747-76E0-D749-A511-4A5793808055}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1509,7 +1784,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1564,7 +1839,7 @@
       </c>
       <c r="D3" s="27">
         <f>params!J4</f>
-        <v>43831</v>
+        <v>44562</v>
       </c>
       <c r="E3" t="str">
         <f>params!M4</f>
@@ -1669,7 +1944,7 @@
       </c>
       <c r="B9">
         <f>params!F10</f>
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C9">
         <f>params!K10</f>
@@ -1681,7 +1956,7 @@
       </c>
       <c r="E9" t="str">
         <f>params!M10</f>
-        <v>Missing</v>
+        <v>Informed guess</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1717,7 +1992,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>params!A15</f>
+        <f>params!A17</f>
         <v>daily_audience</v>
       </c>
       <c r="B14">
@@ -1725,11 +2000,11 @@
         <v>50700000</v>
       </c>
       <c r="C14">
-        <f>params!K15</f>
+        <f>params!K17</f>
         <v>0</v>
       </c>
       <c r="D14" s="27">
-        <f>params!J15</f>
+        <f>params!J17</f>
         <v>43862</v>
       </c>
       <c r="E14" t="str">
@@ -1740,51 +2015,51 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>params!A16</f>
+        <f>params!A18</f>
         <v>daily_viewing_time</v>
       </c>
       <c r="B15">
-        <f>params!F16</f>
+        <f>params!F18</f>
         <v>43</v>
       </c>
       <c r="C15" t="str">
-        <f>params!K16</f>
+        <f>params!K18</f>
         <v>minute</v>
       </c>
       <c r="D15" s="27">
-        <f>params!J16</f>
-        <v>43862</v>
+        <f>params!J18</f>
+        <v>44228</v>
       </c>
       <c r="E15" t="str">
-        <f>params!M16</f>
-        <v>https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/</v>
+        <f>params!M18</f>
+        <v>https://www.ofcom.org.uk/__data/assets/pdf_file/0016/242701/media-nations-report-2022.pdf</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>params!A17</f>
+        <f>params!A19</f>
         <v>bitrate</v>
       </c>
       <c r="B16">
-        <f>params!F17</f>
-        <v>10000000</v>
+        <f>params!F19</f>
+        <v>1688000</v>
       </c>
       <c r="C16" t="str">
-        <f>params!K17</f>
+        <f>params!K19</f>
         <v>bps</v>
       </c>
       <c r="D16" s="27">
-        <f>params!J17</f>
-        <v>43862</v>
+        <f>params!J19</f>
+        <v>44593</v>
       </c>
       <c r="E16" t="str">
-        <f>params!M17</f>
-        <v>https://www.howtogeek.com/338983/how-much-data-does-netflix-use/</v>
+        <f>params!M19</f>
+        <v>Own</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>params!A19</f>
+        <f>params!A21</f>
         <v>power_decoding</v>
       </c>
       <c r="B17" t="e">
@@ -1792,37 +2067,37 @@
         <v>#REF!</v>
       </c>
       <c r="C17" t="str">
-        <f>params!K19</f>
+        <f>params!K21</f>
         <v>W</v>
       </c>
       <c r="D17" s="27">
-        <f>params!J19</f>
+        <f>params!J21</f>
         <v>43862</v>
       </c>
       <c r="E17" t="str">
-        <f>params!M19</f>
+        <f>params!M21</f>
         <v>Missing</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>params!A21</f>
+        <f>params!A23</f>
         <v>0</v>
       </c>
       <c r="B18">
-        <f>params!F21</f>
+        <f>params!F23</f>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>params!K21</f>
+        <f>params!K23</f>
         <v>0</v>
       </c>
       <c r="D18" s="27">
-        <f>params!J21</f>
+        <f>params!J23</f>
         <v>0</v>
       </c>
       <c r="E18">
-        <f>params!M21</f>
+        <f>params!M23</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
README and CITATION added
</commit_message>
<xml_diff>
--- a/short_term_model.xlsx
+++ b/short_term_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Luke Benson\Documents\4th_year\Individual Project\ICIP2023-EAM-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/eam/ICIP2023-EAM-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0A4CC7-21AB-4C0D-BC96-046DD10B8B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC128D7-35E7-0840-A410-0A420A793D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="740" windowWidth="30240" windowHeight="20640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -40,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="166">
   <si>
     <t>variable</t>
   </si>
@@ -214,16 +236,7 @@
     <t>bps</t>
   </si>
   <si>
-    <t>reference</t>
-  </si>
-  <si>
     <t>s720</t>
-  </si>
-  <si>
-    <t>parameter</t>
-  </si>
-  <si>
-    <t>OpenConnect Appliances. https://openconnect.netflix.com/en_gb/appliances/ - lists ideal energy intensity values during full utilisation. From the list of appliances we cautiously select the least energy efficient one (15J/Gb) and double the intensity to account for periods of low utilisation.</t>
   </si>
   <si>
     <t>Combined Cycle Gas. -https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf</t>
@@ -257,10 +270,6 @@
     <t>laptop share</t>
   </si>
   <si>
-    <t xml:space="preserve"> Comscore’s The US Total Video
-Report (Comscore, 2014)</t>
-  </si>
-  <si>
     <t>S/B VoD daily audience</t>
   </si>
   <si>
@@ -268,9 +277,6 @@
 Report (Comscore, 2014)]</t>
   </si>
   <si>
-    <t>Informed guess</t>
-  </si>
-  <si>
     <t>seconds</t>
   </si>
   <si>
@@ -470,6 +476,95 @@
   </si>
   <si>
     <t>t_09</t>
+  </si>
+  <si>
+    <t>P_DC</t>
+  </si>
+  <si>
+    <t>Wh/hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage change: </t>
+  </si>
+  <si>
+    <t>=&gt; saving on laptop is 65x that on the streaming server</t>
+  </si>
+  <si>
+    <t>I_x</t>
+  </si>
+  <si>
+    <t>J/Gb</t>
+  </si>
+  <si>
+    <t>energy at 7500 kbps</t>
+  </si>
+  <si>
+    <t>Wh</t>
+  </si>
+  <si>
+    <t>dv @ 7.5Mbps</t>
+  </si>
+  <si>
+    <t>kbps</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>dv</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>power at 7.5Mbps</t>
+  </si>
+  <si>
+    <t>I_linode</t>
+  </si>
+  <si>
+    <t>J/b</t>
+  </si>
+  <si>
+    <t>https://www.vox.com/2018/3/7/17094610/netflix-70-percent-tv-viewing-statistics</t>
+  </si>
+  <si>
+    <t>Paul shared 20.02- --" biggest delta"</t>
+  </si>
+  <si>
+    <t>https://support.google.com/interconnect/answer/9058809?hl=en</t>
+  </si>
+  <si>
+    <t>0.0301 Wh/30min = 0.0602 Wh/h = 0.06 W ;; https://www.datacenterknowledge.com/energy/how-much-netflix-really-contributing-climate-change ;;
+46% of 0.06W =&gt; 0.0276W
+Curious: Netflix "fills" from 2am to 2pm.</t>
+  </si>
+  <si>
+    <t>OpenConnect Appliances. https://openconnect.netflix.com/en_gb/appliances/ - lists ideal energy intensity values during full utilisation. From the list of appliances we calculate the marginal energy intensity, assuming 40% base power and PUE of 1.5. Cautiously select the least energy efficient one (9J/Gb).</t>
+  </si>
+  <si>
+    <t>PUE</t>
+  </si>
+  <si>
+    <t>Bianco et al. https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=7511356</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Marginal by slope</t>
   </si>
 </sst>
 </file>
@@ -477,11 +572,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -583,7 +678,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -609,7 +704,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,6 +747,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -690,11 +791,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -719,7 +820,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -783,8 +884,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -796,12 +897,23 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -887,7 +999,330 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>carbon_intensity!$N$2:$N$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>272.552055</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>266.00684899999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>248.772603</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>248.97123300000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285.236986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>334.45890400000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>334.44383599999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>239.157534</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>151.635616</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>102.39588999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>118.893151</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148.57671199999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>202.276712</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>154.60137</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>124.07123300000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>208.64657500000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>177.21643800000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>121.783562</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>147.079452</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>175.157534</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>297.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>376.54520500000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>382.26712300000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>360.48767099999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECEC-EC49-8F3D-BCE935E9F479}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1348608464"/>
+        <c:axId val="1349190752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1348608464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1349190752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1349190752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1348608464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1292,10 +1727,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1793,10 +2228,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2285,6 +2720,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3833,7 +4308,613 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>872434</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>905013</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>45278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29944F37-5FA5-85B8-C7E4-0A0B948C49DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17095304" y="2396435"/>
+          <a:ext cx="7277100" cy="5003800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20671CE-E1C2-479D-D524-5D98EB1F75AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4287,24 +5368,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.6640625" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="59.44140625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="59.5" hidden="1" customWidth="1"/>
     <col min="20" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4372,7 +5455,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="45"/>
       <c r="B2" s="44" t="s">
         <v>17</v>
@@ -4392,41 +5475,37 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
     </row>
-    <row r="3" spans="1:22" ht="16.95" customHeight="1">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:22" ht="112" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="4"/>
+      <c r="F3" s="38">
+        <f>0.000000281*1000000000</f>
+        <v>281</v>
+      </c>
+      <c r="K3" t="s">
+        <v>63</v>
+      </c>
       <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="31"/>
-      <c r="Q3" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="M3" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+    <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32">
-        <v>30</v>
-      </c>
-      <c r="G4" s="33">
-        <v>-0.2</v>
-      </c>
+      <c r="F4" s="14">
+        <v>1.3</v>
+      </c>
+      <c r="G4" s="19"/>
       <c r="H4" s="33">
         <v>0.1</v>
       </c>
@@ -4434,42 +5513,44 @@
         <v>0.05</v>
       </c>
       <c r="J4" s="34">
-        <v>44562</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="32"/>
-      <c r="Q4" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="45"/>
+        <v>43831</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="31"/>
+      <c r="Q4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="32"/>
+      <c r="F5" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="31"/>
+      <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:22" ht="19.95" customHeight="1">
+      <c r="S5" s="6"/>
+    </row>
+    <row r="6" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
@@ -4478,52 +5559,57 @@
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="32">
-        <v>0.03</v>
-      </c>
-      <c r="G6" s="32">
-        <v>0</v>
-      </c>
-      <c r="H6" s="32">
+        <f>9*F5</f>
+        <v>13.5</v>
+      </c>
+      <c r="G6" s="33">
+        <v>-0.2</v>
+      </c>
+      <c r="H6" s="33">
         <v>0.1</v>
       </c>
       <c r="I6" s="33">
         <v>0.05</v>
       </c>
       <c r="J6" s="34">
-        <v>43831</v>
+        <v>44562</v>
       </c>
       <c r="K6" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L6" s="32"/>
-      <c r="M6" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="M6" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="N6" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="35"/>
-    </row>
-    <row r="8" spans="1:22" ht="22.95" customHeight="1">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="45"/>
+      <c r="B7" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="45"/>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -4532,7 +5618,7 @@
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="32">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G8" s="32">
         <v>-0.2</v>
@@ -4544,95 +5630,101 @@
         <v>0.05</v>
       </c>
       <c r="J8" s="34">
-        <v>43831</v>
+        <v>43983</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="4"/>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="1:22" ht="28.8">
-      <c r="A10" s="13" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="35"/>
+    </row>
+    <row r="10" spans="1:22" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32">
+        <v>0.02</v>
+      </c>
+      <c r="G10" s="49">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="J10" s="34">
+        <v>43831</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="32"/>
+      <c r="M10" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="4"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" ht="80" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16">
-        <v>0.05</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="J10" s="20">
-        <v>43831</v>
-      </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="18"/>
-      <c r="Q10" s="22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="45"/>
-      <c r="B11" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="1:22" ht="24" customHeight="1">
-      <c r="A12" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="14">
-        <v>394</v>
-      </c>
-      <c r="G12" s="19">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="21">
         <v>0</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="14">
         <v>0.1</v>
       </c>
       <c r="I12" s="19">
@@ -4641,150 +5733,130 @@
       <c r="J12" s="20">
         <v>43831</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>130</v>
-      </c>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q12" t="s">
+        <v>156</v>
+      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="18"/>
+      <c r="Q12" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="45"/>
+      <c r="B13" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="14">
+        <v>394</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="20">
+        <v>43831</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" t="s">
         <v>25</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
-      <c r="F13" s="14"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-      <c r="Q13" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="F15" s="14"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="Q15" t="s">
         <v>26</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
-      <c r="E14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:22" ht="34.049999999999997" customHeight="1">
-      <c r="D15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="28">
-        <v>50700000</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="M15" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="P15" s="48" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="25.05" customHeight="1">
-      <c r="D16" s="13" t="s">
-        <v>70</v>
-      </c>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="E16" s="13"/>
-      <c r="F16" s="37">
-        <v>0.12</v>
-      </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-      <c r="M16" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="P16" s="48" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="34.049999999999997" customHeight="1">
-      <c r="A17" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="38">
-        <f>F15*F16</f>
-        <v>6084000</v>
-      </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="I17" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="J17" s="20">
-        <v>43862</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="M17" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="P17" s="48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="31.05" customHeight="1">
-      <c r="A18" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
+    </row>
+    <row r="17" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="28">
+        <v>50700000</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="M17" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="17"/>
+    </row>
+    <row r="18" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="15">
-        <v>43</v>
-      </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="I18" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="J18" s="20">
-        <v>44228</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M18" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="P18" s="48" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="34.950000000000003" customHeight="1">
-      <c r="A19" t="s">
-        <v>40</v>
+      <c r="F18" s="37">
+        <v>0.15</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="M18" s="53" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="38">
-        <v>1688000</v>
+        <f>F17*F18</f>
+        <v>7605000</v>
       </c>
       <c r="G19" s="19">
         <v>0</v>
@@ -4796,33 +5868,23 @@
         <v>0.05</v>
       </c>
       <c r="J19" s="20">
-        <v>44593</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="M19" s="30" t="s">
+        <v>43862</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="M19" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="P19" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.6">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>58</v>
+    </row>
+    <row r="20" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="38">
-        <v>911000</v>
+      <c r="E20" s="13"/>
+      <c r="F20" s="15">
+        <v>42</v>
       </c>
       <c r="G20" s="19">
         <v>0</v>
@@ -4834,25 +5896,25 @@
         <v>0.05</v>
       </c>
       <c r="J20" s="20">
-        <v>44593</v>
+        <v>44228</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="M20" s="5"/>
-      <c r="P20" s="48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="43.2">
+        <v>60</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="17"/>
+    </row>
+    <row r="21" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="F21">
-        <v>6.6023598758794488</v>
+      <c r="F21" s="38">
+        <v>1688000</v>
       </c>
       <c r="G21" s="19">
         <v>0</v>
@@ -4864,30 +5926,33 @@
         <v>0.05</v>
       </c>
       <c r="J21" s="20">
-        <v>43862</v>
-      </c>
-      <c r="K21" t="s">
-        <v>43</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="P21" s="48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.6">
+        <v>44593</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="F22">
-        <v>4.7998260991263555</v>
+      <c r="F22" s="38">
+        <v>911000</v>
       </c>
       <c r="G22" s="19">
         <v>0</v>
@@ -4899,257 +5964,375 @@
         <v>0.05</v>
       </c>
       <c r="J22" s="20">
-        <v>43862</v>
+        <v>44593</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="M22" s="5"/>
-      <c r="P22" s="48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.6">
-      <c r="F23" s="14"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="M23" s="5"/>
-      <c r="P23" s="48" t="s">
+      <c r="N22">
+        <f>(F21-F22)/F21</f>
+        <v>0.46030805687203791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23">
+        <v>6.6023598758794488</v>
+      </c>
+      <c r="G23" s="19">
+        <v>0</v>
+      </c>
+      <c r="H23" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I23" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="J23" s="20">
+        <v>44593</v>
+      </c>
+      <c r="K23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N23">
+        <f>F23-F24</f>
+        <v>1.8025337767530933</v>
+      </c>
+      <c r="P23" s="17"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>4.7998260991263555</v>
+      </c>
+      <c r="G24" s="19">
+        <v>0</v>
+      </c>
+      <c r="H24" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I24" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="J24" s="20">
+        <v>44593</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24">
+        <f>N23/0.0276</f>
+        <v>65.309194809894692</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F25" s="14"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="52" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.6">
-      <c r="B24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="20"/>
-      <c r="P24" s="48" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="13"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="P26" s="17"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="47"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="39">
+        <f>F19*F20*60</f>
+        <v>19164600000</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="K29">
+        <v>469.40175416605479</v>
+      </c>
+      <c r="P29" s="17"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
+      <c r="E30" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="39">
+        <f>F29*365/12</f>
+        <v>582923250000</v>
+      </c>
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="K30">
+        <v>9857.4368374871538</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="13"/>
+      <c r="D31">
+        <v>1080</v>
+      </c>
+      <c r="J31" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="K31">
+        <v>6720.6160710000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E32" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="39">
+        <f>F30*F23</f>
+        <v>3848669076517.2451</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="K32">
+        <v>4316.8420481675757</v>
+      </c>
+      <c r="P32" s="17"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="39">
+        <f>F32/3600000</f>
+        <v>1069074.7434770125</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J33" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33">
+        <v>876222.86509401642</v>
+      </c>
+      <c r="L33" s="39">
+        <f>K33/F33</f>
+        <v>0.81960861056751466</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E34" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="39">
+        <f>F33*F14</f>
+        <v>421215448.92994291</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P35" s="17"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E36" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="39">
+        <f>F21*F30</f>
+        <v>9.83974446E+17</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F37" s="39">
+        <f>F36/1000000</f>
+        <v>983974446000</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E38" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F38" s="39">
+        <f>F37*F10</f>
+        <v>19679488920</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="P38" s="17"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F39" s="39">
+        <f>F38/3600000</f>
+        <v>5466.5246999999999</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P41" s="17"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K47" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.6">
-      <c r="P25" s="48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="15.6">
-      <c r="A26" s="47"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="P26" s="48" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.6">
-      <c r="A27" s="13"/>
-      <c r="E27" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="39">
-        <f>F17*F18*60</f>
-        <v>15696720000</v>
-      </c>
-      <c r="G27" t="s">
-        <v>75</v>
-      </c>
-      <c r="J27" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="K27">
-        <v>469.40175416605479</v>
-      </c>
-      <c r="P27" s="48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.6">
-      <c r="A28" s="13"/>
-      <c r="E28" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="39">
-        <f>F27*365/12</f>
-        <v>477441900000</v>
-      </c>
-      <c r="G28" t="s">
-        <v>75</v>
-      </c>
-      <c r="J28" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="K28">
-        <v>9857.4368374871538</v>
-      </c>
-      <c r="P28" s="48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="15.6">
-      <c r="A29" s="13"/>
-      <c r="D29">
-        <v>1080</v>
-      </c>
-      <c r="J29" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="K29">
-        <v>6720.6160710000004</v>
-      </c>
-      <c r="P29" s="48" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.6">
-      <c r="E30" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="39">
-        <f>F28*F21</f>
-        <v>3152243243623.6484</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="J30" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="K30">
-        <v>4316.8420481675757</v>
-      </c>
-      <c r="P30" s="48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.6">
-      <c r="A31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="39">
-        <f>F30/3600000</f>
-        <v>875623.12322879129</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J31" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="K31">
-        <v>876222.86509401642</v>
-      </c>
-      <c r="L31" s="39">
-        <f>K31/F31</f>
-        <v>1.0006849315068493</v>
-      </c>
-      <c r="P31" s="48" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.6">
-      <c r="E32" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" s="39">
-        <f>F31*F12</f>
-        <v>344995510.55214375</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="P32" s="48" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="5:16" ht="15.6">
-      <c r="P33" s="48" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="5:16" ht="15.6">
-      <c r="E34" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="39">
-        <f>F19*F28</f>
-        <v>8.059219272E+17</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="P34" s="48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="5:16" ht="15.6">
-      <c r="F35" s="39">
-        <f>F34/1000000</f>
-        <v>805921927200</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="P35" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="5:16" ht="15.6">
-      <c r="E36" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="39">
-        <f>F35*F8</f>
-        <v>16118438544</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="P36" s="48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="5:16" ht="15.6">
-      <c r="F37" s="39">
-        <f>F36/3600000</f>
-        <v>4477.3440399999999</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="P37" s="48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="5:16" ht="15.6">
-      <c r="P38" s="48" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="5:16">
-      <c r="P39" s="17">
-        <v>24</v>
+      <c r="L47">
+        <v>30</v>
+      </c>
+      <c r="M47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="K49" t="s">
+        <v>143</v>
+      </c>
+      <c r="L49">
+        <v>0.06</v>
+      </c>
+      <c r="M49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="K50" t="s">
+        <v>151</v>
+      </c>
+      <c r="L50">
+        <v>0.06</v>
+      </c>
+      <c r="M50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J52" t="s">
+        <v>145</v>
+      </c>
+      <c r="K52" t="s">
+        <v>40</v>
+      </c>
+      <c r="L52">
+        <v>7500</v>
+      </c>
+      <c r="M52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="K53" t="s">
+        <v>147</v>
+      </c>
+      <c r="L53">
+        <v>3600</v>
+      </c>
+      <c r="M53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="K54" t="s">
+        <v>149</v>
+      </c>
+      <c r="L54">
+        <f>L53*L52*1000</f>
+        <v>27000000000</v>
+      </c>
+      <c r="M54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="K56" t="s">
+        <v>152</v>
+      </c>
+      <c r="L56">
+        <f>L50/L54</f>
+        <v>2.222222222222222E-12</v>
+      </c>
+      <c r="M56" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <f>L56*1000000000</f>
+        <v>2.2222222222222218E-3</v>
+      </c>
+      <c r="M57" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q10" r:id="rId1" xr:uid="{9457789D-A2B4-684F-8723-371AC82363FD}"/>
-    <hyperlink ref="Q4" r:id="rId2" xr:uid="{770F17AD-6F52-D749-93D4-3560E5A28FFE}"/>
-    <hyperlink ref="M12" r:id="rId3" display="https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf" xr:uid="{F9266DB3-7397-8F48-83F2-55D825A1A6CA}"/>
-    <hyperlink ref="M18" r:id="rId4" xr:uid="{13F557E0-5A18-8140-A2C7-150350381894}"/>
-    <hyperlink ref="M15" r:id="rId5" display="https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/_x000a__x000a_Ofcom finds the viewing time has remained largely similar since pandemic ()" xr:uid="{78A7B747-76E0-D749-A511-4A5793808055}"/>
+    <hyperlink ref="Q12" r:id="rId1" xr:uid="{9457789D-A2B4-684F-8723-371AC82363FD}"/>
+    <hyperlink ref="Q6" r:id="rId2" xr:uid="{770F17AD-6F52-D749-93D4-3560E5A28FFE}"/>
+    <hyperlink ref="M14" r:id="rId3" display="https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf" xr:uid="{F9266DB3-7397-8F48-83F2-55D825A1A6CA}"/>
+    <hyperlink ref="M20" r:id="rId4" xr:uid="{13F557E0-5A18-8140-A2C7-150350381894}"/>
+    <hyperlink ref="M17" r:id="rId5" display="https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/_x000a__x000a_Ofcom finds the viewing time has remained largely similar since pandemic ()" xr:uid="{78A7B747-76E0-D749-A511-4A5793808055}"/>
+    <hyperlink ref="M18" r:id="rId6" xr:uid="{3A3EDA19-6F7F-2B4B-BD04-E37AF44B0EAA}"/>
+    <hyperlink ref="M12" r:id="rId7" xr:uid="{9831A1D9-2E54-E24C-A8A5-B6FF3B97EE2D}"/>
+    <hyperlink ref="M3" r:id="rId8" display="https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=7511356" xr:uid="{DEDDA21B-96C0-1849-AF53-3438B0E54F57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -5158,14 +6341,14 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C2" sqref="C2:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5183,196 +6366,196 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2">
+        <v>1.4168554229999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3">
+        <v>0.63783970300000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4">
+        <v>0.37404512000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>0.31920586299999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6">
+        <v>0.26436660499999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="C2">
-        <v>1.4168554230491466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6">
-      <c r="A3" s="48" t="s">
+      <c r="C7">
+        <v>0.29876190600000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C3">
-        <v>0.63783970344165508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6">
-      <c r="A4" s="48" t="s">
+      <c r="C8">
+        <v>0.86660710100000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="C4">
-        <v>0.37404512026568548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6">
-      <c r="A5" s="48" t="s">
+      <c r="C9">
+        <v>1.514157964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="C5">
-        <v>0.31920586258595213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.6">
-      <c r="A6" s="48" t="s">
+      <c r="C10">
+        <v>1.7012569230000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="C6">
-        <v>0.26436660490621872</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.6">
-      <c r="A7" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7">
-        <v>0.29876190571814276</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6">
-      <c r="A8" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8">
-        <v>0.86660710133624186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.6">
-      <c r="A9" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9">
-        <v>1.5141579637419422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.6">
-      <c r="A10" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10">
-        <v>1.7012569227718957</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.6">
-      <c r="A11" s="48" t="s">
-        <v>141</v>
-      </c>
       <c r="C11">
-        <v>1.6595511620760224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.6">
+        <v>1.6595511620000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>1.5244268249999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13">
+        <v>1.448150056</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14">
+        <v>1.575906287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15">
+        <v>1.7089537189999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16">
+        <v>1.593198581</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="C12">
-        <v>1.5244268254168198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.6">
-      <c r="A13" s="48" t="s">
+      <c r="C17">
+        <v>1.802996974</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="C13">
-        <v>1.4481500556837466</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.6">
-      <c r="A14" s="48" t="s">
+      <c r="C18">
+        <v>2.169305574</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="C14">
-        <v>1.5759062868582798</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.6">
-      <c r="A15" s="48" t="s">
+      <c r="C19">
+        <v>2.535614174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="C15">
-        <v>1.7089537190376094</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.6">
-      <c r="A16" s="48" t="s">
+      <c r="C20">
+        <v>2.9019227750000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="C16">
-        <v>1.593198581363509</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.6">
-      <c r="A17" s="48" t="s">
+      <c r="C21">
+        <v>3.188140942</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="C17">
-        <v>1.8029969737703151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.6">
-      <c r="A18" s="48" t="s">
+      <c r="C22">
+        <v>3.4647006999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="C18">
-        <v>2.1693055740390208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.6">
-      <c r="A19" s="48" t="s">
+      <c r="C23">
+        <v>3.4224707250000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C19">
-        <v>2.5356141743077263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.6">
-      <c r="A20" s="48" t="s">
+      <c r="C24">
+        <v>3.5257825880000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C20">
-        <v>2.9019227745764318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.6">
-      <c r="A21" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21">
-        <v>3.1881409421488738</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.6">
-      <c r="A22" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22">
-        <v>3.464700700177167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.6">
-      <c r="A23" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23">
-        <v>3.4224707247997266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.6">
-      <c r="A24" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24">
-        <v>3.5257825884159235</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.6">
-      <c r="A25" s="48" t="s">
-        <v>128</v>
-      </c>
       <c r="C25">
-        <v>3.0857823095119334</v>
+        <v>3.0857823099999999</v>
       </c>
     </row>
   </sheetData>
@@ -5382,17 +6565,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6A4CB5-69F6-F447-81D4-FE2367EAF2AB}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5410,205 +6593,621 @@
         <v>8</v>
       </c>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6">
+      <c r="M1" t="s">
+        <v>155</v>
+      </c>
+      <c r="R1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" cm="1">
+        <f t="array" ref="C2:C25">S2:S25</f>
+        <v>280</v>
+      </c>
+      <c r="M2">
+        <v>0.27255205500000002</v>
+      </c>
+      <c r="N2">
+        <f>M2*1000</f>
+        <v>272.552055</v>
+      </c>
+      <c r="P2" s="43">
+        <v>161.8295019</v>
+      </c>
+      <c r="R2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S2">
+        <f>R2*1000</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3">
+        <v>408</v>
+      </c>
+      <c r="M3">
+        <v>0.26600684899999999</v>
+      </c>
+      <c r="N3">
+        <f>M3*1000</f>
+        <v>266.00684899999999</v>
+      </c>
+      <c r="P3" s="43">
+        <v>160.9808429</v>
+      </c>
+      <c r="R3">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S25" si="0">R3*1000</f>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4">
+        <v>232</v>
+      </c>
+      <c r="M4">
+        <v>0.24877260300000001</v>
+      </c>
+      <c r="N4">
+        <f>M4*1000</f>
+        <v>248.772603</v>
+      </c>
+      <c r="P4" s="43">
+        <v>159.10153260000001</v>
+      </c>
+      <c r="R4">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>190</v>
+      </c>
+      <c r="M5">
+        <v>0.24897123300000001</v>
+      </c>
+      <c r="N5">
+        <f>M5*1000</f>
+        <v>248.97123300000001</v>
+      </c>
+      <c r="P5" s="43">
+        <v>158.9961686</v>
+      </c>
+      <c r="R5">
+        <v>0.19</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6">
+        <v>195</v>
+      </c>
+      <c r="M6">
+        <v>0.28523698600000003</v>
+      </c>
+      <c r="N6">
+        <f>M6*1000</f>
+        <v>285.236986</v>
+      </c>
+      <c r="P6" s="43">
+        <v>163.4291188</v>
+      </c>
+      <c r="R6">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43">
-        <v>161.8295019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.6">
-      <c r="A3" s="48" t="s">
+      <c r="C7">
+        <v>333</v>
+      </c>
+      <c r="M7">
+        <v>0.334458904</v>
+      </c>
+      <c r="N7">
+        <f>M7*1000</f>
+        <v>334.45890400000002</v>
+      </c>
+      <c r="P7" s="43">
+        <v>177.37931029999999</v>
+      </c>
+      <c r="R7">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="43">
-        <v>160.9808429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.6">
-      <c r="A4" s="48" t="s">
+      <c r="C8">
+        <v>416</v>
+      </c>
+      <c r="M8">
+        <v>0.33444383599999999</v>
+      </c>
+      <c r="N8">
+        <f>M8*1000</f>
+        <v>334.44383599999998</v>
+      </c>
+      <c r="P8" s="43">
+        <v>194.62068970000001</v>
+      </c>
+      <c r="R8">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="43">
-        <v>159.10153260000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6">
-      <c r="A5" s="48" t="s">
+      <c r="C9">
+        <v>395</v>
+      </c>
+      <c r="M9">
+        <v>0.239157534</v>
+      </c>
+      <c r="N9">
+        <f>M9*1000</f>
+        <v>239.157534</v>
+      </c>
+      <c r="P9" s="43">
+        <v>202.58237550000001</v>
+      </c>
+      <c r="R9">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="43">
-        <v>158.9961686</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6">
-      <c r="A6" s="48" t="s">
+      <c r="C10">
+        <v>224</v>
+      </c>
+      <c r="M10">
+        <v>0.151635616</v>
+      </c>
+      <c r="N10">
+        <f>M10*1000</f>
+        <v>151.635616</v>
+      </c>
+      <c r="P10" s="43">
+        <v>200.98659000000001</v>
+      </c>
+      <c r="R10">
+        <v>0.224</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="43">
-        <v>163.4291188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6">
-      <c r="A7" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="43">
-        <v>177.37931029999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.6">
-      <c r="A8" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="43">
-        <v>194.62068970000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.6">
-      <c r="A9" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="43">
-        <v>202.58237550000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.6">
-      <c r="A10" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="43">
-        <v>200.98659000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6">
-      <c r="A11" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="C11" s="43">
+      <c r="C11">
+        <v>162</v>
+      </c>
+      <c r="M11">
+        <v>0.10239588999999999</v>
+      </c>
+      <c r="N11">
+        <f>M11*1000</f>
+        <v>102.39588999999999</v>
+      </c>
+      <c r="P11" s="43">
         <v>196.61111109999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.6">
+      <c r="R11">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>309</v>
+      </c>
+      <c r="M12">
+        <v>0.118893151</v>
+      </c>
+      <c r="N12">
+        <f>M12*1000</f>
+        <v>118.893151</v>
+      </c>
+      <c r="P12" s="43">
+        <v>191.38505749999999</v>
+      </c>
+      <c r="R12">
+        <v>0.309</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13">
+        <v>253</v>
+      </c>
+      <c r="M13">
+        <v>0.148576712</v>
+      </c>
+      <c r="N13">
+        <f>M13*1000</f>
+        <v>148.57671199999999</v>
+      </c>
+      <c r="P13" s="43">
+        <v>188.39463599999999</v>
+      </c>
+      <c r="R13">
+        <v>0.253</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14">
+        <v>281</v>
+      </c>
+      <c r="M14">
+        <v>0.202276712</v>
+      </c>
+      <c r="N14">
+        <f>M14*1000</f>
+        <v>202.276712</v>
+      </c>
+      <c r="P14" s="43">
+        <v>186.1896552</v>
+      </c>
+      <c r="R14">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15">
+        <v>188</v>
+      </c>
+      <c r="M15">
+        <v>0.15460137000000002</v>
+      </c>
+      <c r="N15">
+        <f>M15*1000</f>
+        <v>154.60137</v>
+      </c>
+      <c r="P15" s="43">
+        <v>185.6743295</v>
+      </c>
+      <c r="R15">
+        <v>0.188</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="M16">
+        <v>0.124071233</v>
+      </c>
+      <c r="N16">
+        <f>M16*1000</f>
+        <v>124.07123300000001</v>
+      </c>
+      <c r="P16" s="43">
+        <v>189.98659000000001</v>
+      </c>
+      <c r="R16">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="43">
-        <v>191.38505749999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.6">
-      <c r="A13" s="48" t="s">
+      <c r="C17">
+        <v>259</v>
+      </c>
+      <c r="M17">
+        <v>0.208646575</v>
+      </c>
+      <c r="N17">
+        <f>M17*1000</f>
+        <v>208.64657500000001</v>
+      </c>
+      <c r="P17" s="43">
+        <v>198.83716480000001</v>
+      </c>
+      <c r="R17">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="43">
-        <v>188.39463599999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.6">
-      <c r="A14" s="48" t="s">
+      <c r="C18">
+        <v>417</v>
+      </c>
+      <c r="M18">
+        <v>0.177216438</v>
+      </c>
+      <c r="N18">
+        <f>M18*1000</f>
+        <v>177.21643800000001</v>
+      </c>
+      <c r="P18" s="43">
+        <v>206.66666670000001</v>
+      </c>
+      <c r="R18">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="0"/>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="43">
-        <v>186.1896552</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.6">
-      <c r="A15" s="48" t="s">
+      <c r="C19">
+        <v>258</v>
+      </c>
+      <c r="M19">
+        <v>0.121783562</v>
+      </c>
+      <c r="N19">
+        <f>M19*1000</f>
+        <v>121.783562</v>
+      </c>
+      <c r="P19" s="43">
+        <v>211.86973180000001</v>
+      </c>
+      <c r="R19">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="43">
-        <v>185.6743295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.6">
-      <c r="A16" s="48" t="s">
+      <c r="C20">
+        <v>245</v>
+      </c>
+      <c r="M20">
+        <v>0.147079452</v>
+      </c>
+      <c r="N20">
+        <f>M20*1000</f>
+        <v>147.079452</v>
+      </c>
+      <c r="P20" s="43">
+        <v>215.1091954</v>
+      </c>
+      <c r="R20">
+        <v>0.245</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="0"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="43">
-        <v>189.98659000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.6">
-      <c r="A17" s="48" t="s">
+      <c r="C21">
+        <v>248</v>
+      </c>
+      <c r="M21">
+        <v>0.175157534</v>
+      </c>
+      <c r="N21">
+        <f>M21*1000</f>
+        <v>175.157534</v>
+      </c>
+      <c r="P21" s="43">
+        <v>216.75287359999999</v>
+      </c>
+      <c r="R21">
+        <v>0.248</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="43">
-        <v>198.83716480000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.6">
-      <c r="A18" s="48" t="s">
+      <c r="C22">
+        <v>340</v>
+      </c>
+      <c r="M22">
+        <v>0.29710000000000003</v>
+      </c>
+      <c r="N22">
+        <f>M22*1000</f>
+        <v>297.10000000000002</v>
+      </c>
+      <c r="P22" s="43">
+        <v>211.82183910000001</v>
+      </c>
+      <c r="R22">
+        <v>0.34</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="43">
-        <v>206.66666670000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.6">
-      <c r="A19" s="48" t="s">
+      <c r="C23">
+        <v>507</v>
+      </c>
+      <c r="M23">
+        <v>0.37654520499999999</v>
+      </c>
+      <c r="N23">
+        <f>M23*1000</f>
+        <v>376.54520500000001</v>
+      </c>
+      <c r="P23" s="43">
+        <v>198.18773949999999</v>
+      </c>
+      <c r="R23">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="0"/>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="43">
-        <v>211.86973180000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.6">
-      <c r="A20" s="48" t="s">
+      <c r="C24">
+        <v>359</v>
+      </c>
+      <c r="M24">
+        <v>0.38226712300000004</v>
+      </c>
+      <c r="N24">
+        <f>M24*1000</f>
+        <v>382.26712300000003</v>
+      </c>
+      <c r="P24" s="43">
+        <v>180.302682</v>
+      </c>
+      <c r="R24">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="0"/>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="43">
-        <v>215.1091954</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.6">
-      <c r="A21" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="43">
-        <v>216.75287359999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.6">
-      <c r="A22" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="43">
-        <v>211.82183910000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.6">
-      <c r="A23" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="43">
-        <v>198.18773949999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.6">
-      <c r="A24" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="43">
-        <v>180.302682</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.6">
-      <c r="A25" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="43">
+      <c r="C25">
+        <v>326</v>
+      </c>
+      <c r="M25">
+        <v>0.36048767099999995</v>
+      </c>
+      <c r="N25">
+        <f>M25*1000</f>
+        <v>360.48767099999998</v>
+      </c>
+      <c r="P25" s="43">
         <v>166.66091950000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.6">
+      <c r="R25">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5617,388 +7216,312 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F17" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>164</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <f>params!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>params!F3</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>params!K3</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="27">
-        <f>params!J3</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>params!M3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>params!A4</f>
+        <f>params!A6</f>
         <v>I_Tx</v>
       </c>
       <c r="B3">
-        <f>params!F4</f>
-        <v>30</v>
+        <f>params!F6</f>
+        <v>13.5</v>
       </c>
       <c r="C3" t="str">
-        <f>params!K4</f>
+        <f>params!K6</f>
         <v>J/gigabit</v>
       </c>
       <c r="D3" s="27">
-        <f>params!J4</f>
+        <f>params!J6</f>
         <v>44562</v>
       </c>
       <c r="E3" t="str">
-        <f>params!M4</f>
-        <v>OpenConnect Appliances. https://openconnect.netflix.com/en_gb/appliances/ - lists ideal energy intensity values during full utilisation. From the list of appliances we cautiously select the least energy efficient one (15J/Gb) and double the intensity to account for periods of low utilisation.</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <f>params!M6</f>
+        <v>OpenConnect Appliances. https://openconnect.netflix.com/en_gb/appliances/ - lists ideal energy intensity values during full utilisation. From the list of appliances we calculate the marginal energy intensity, assuming 40% base power and PUE of 1.5. Cautiously select the least energy efficient one (9J/Gb).</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="27"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>params!A6</f>
+        <f>params!A8</f>
         <v>I_Core</v>
       </c>
       <c r="B5">
-        <f>params!F6</f>
+        <f>params!F8</f>
         <v>0.03</v>
       </c>
       <c r="C5" t="str">
-        <f>params!K6</f>
-        <v>J/megabit</v>
-      </c>
-      <c r="D5" s="27">
-        <f>params!J6</f>
-        <v>43831</v>
-      </c>
-      <c r="E5" t="str">
-        <f>params!M6</f>
-        <v>The power consumption of mobile and fixed network data services - The case of streaming video and downloading large files</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <f>params!A7</f>
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <f>params!F7</f>
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <f>params!K7</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="27">
-        <f>params!J7</f>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f>params!M7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="str">
-        <f>params!A8</f>
-        <v>I_Acc</v>
-      </c>
-      <c r="B7">
-        <f>params!F8</f>
-        <v>0.02</v>
-      </c>
-      <c r="C7" t="str">
         <f>params!K8</f>
         <v>J/megabit</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D5" s="27">
         <f>params!J8</f>
-        <v>43831</v>
-      </c>
-      <c r="E7" t="str">
+        <v>43983</v>
+      </c>
+      <c r="E5" t="str">
         <f>params!M8</f>
         <v>The power consumption of mobile and fixed network data services - The case of streaming video and downloading large files</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <f>params!A9</f>
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <f>params!F9</f>
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <f>params!K9</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="27">
-        <f>params!J9</f>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>params!M9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
         <f>params!A10</f>
-        <v>cachemiss_rate</v>
-      </c>
-      <c r="B9">
+        <v>I_Acc</v>
+      </c>
+      <c r="B7">
         <f>params!F10</f>
-        <v>0.05</v>
-      </c>
-      <c r="C9">
+        <v>0.02</v>
+      </c>
+      <c r="C7" t="str">
         <f>params!K10</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="27">
+        <v>J/megabit</v>
+      </c>
+      <c r="D7" s="27">
         <f>params!J10</f>
         <v>43831</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E7" t="str">
         <f>params!M10</f>
-        <v>Informed guess</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="str">
+        <v>The power consumption of mobile and fixed network data services - The case of streaming video and downloading large files</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
         <f>params!A12</f>
-        <v>carbon_intensity</v>
-      </c>
-      <c r="B11">
+        <v>cachemiss_rate</v>
+      </c>
+      <c r="B9">
         <f>params!F12</f>
-        <v>394</v>
-      </c>
-      <c r="C11" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="C9">
         <f>params!K12</f>
-        <v>g/kWh</v>
-      </c>
-      <c r="D11" s="27">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27">
         <f>params!J12</f>
         <v>43831</v>
       </c>
+      <c r="E9" t="str">
+        <f>params!M12</f>
+        <v>https://support.google.com/interconnect/answer/9058809?hl=en</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="27"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>params!A14</f>
+        <v>carbon_intensity</v>
+      </c>
+      <c r="B11">
+        <f>params!F14</f>
+        <v>394</v>
+      </c>
+      <c r="C11" t="str">
+        <f>params!K14</f>
+        <v>g/kWh</v>
+      </c>
+      <c r="D11" s="27">
+        <f>params!J14</f>
+        <v>43831</v>
+      </c>
       <c r="E11" t="str">
-        <f>params!M12</f>
+        <f>params!M14</f>
         <v>Combined Cycle Gas. -https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D12" s="27"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>params!A17</f>
+        <f>params!A19</f>
         <v>daily_audience</v>
       </c>
       <c r="B14">
-        <f>params!F15</f>
+        <f>params!F17</f>
         <v>50700000</v>
       </c>
       <c r="C14">
-        <f>params!K17</f>
+        <f>params!K19</f>
         <v>0</v>
       </c>
       <c r="D14" s="27">
-        <f>params!J17</f>
+        <f>params!J19</f>
         <v>43862</v>
       </c>
       <c r="E14" t="str">
-        <f>params!M15</f>
+        <f>params!M17</f>
         <v>https://www.barb.co.uk/viewing-data/total-identified-viewing-summary/
 Ofcom finds the viewing time has remained largely similar since pandemic (https://www.ofcom.org.uk/__data/assets/pdf_file/0016/242701/media-nations-report-2022.pdf)</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>params!A18</f>
+        <f>params!A20</f>
         <v>viewing_time</v>
       </c>
       <c r="B15">
-        <f>params!F18</f>
-        <v>43</v>
+        <f>params!F20</f>
+        <v>42</v>
       </c>
       <c r="C15" t="str">
-        <f>params!K18</f>
+        <f>params!K20</f>
         <v>minute</v>
       </c>
       <c r="D15" s="27">
-        <f>params!J18</f>
+        <f>params!J20</f>
         <v>44228</v>
       </c>
       <c r="E15" t="str">
-        <f>params!M18</f>
+        <f>params!M20</f>
         <v>https://www.ofcom.org.uk/__data/assets/pdf_file/0016/242701/media-nations-report-2022.pdf</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>params!A19</f>
+        <f>params!A21</f>
         <v>bitrate</v>
       </c>
       <c r="B16">
-        <f>params!F19</f>
+        <f>params!F21</f>
         <v>1688000</v>
       </c>
       <c r="C16" t="str">
-        <f>params!K19</f>
+        <f>params!K21</f>
         <v>bps</v>
       </c>
       <c r="D16" s="27">
-        <f>params!J19</f>
+        <f>params!J21</f>
         <v>44593</v>
       </c>
       <c r="E16" t="str">
-        <f>params!M19</f>
+        <f>params!M21</f>
         <v>Own</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>params!A21</f>
+        <f>params!A23</f>
         <v>power_decoding</v>
       </c>
-      <c r="B17" t="e">
-        <f>params!#REF!</f>
-        <v>#REF!</v>
+      <c r="B17">
+        <f>params!F23</f>
+        <v>6.6023598758794488</v>
       </c>
       <c r="C17" t="str">
-        <f>params!K21</f>
+        <f>params!K23</f>
         <v>W</v>
       </c>
       <c r="D17" s="27">
-        <f>params!J21</f>
-        <v>43862</v>
+        <f>params!J23</f>
+        <v>44593</v>
       </c>
       <c r="E17" t="str">
-        <f>params!M21</f>
+        <f>params!M23</f>
         <v>Own measurements</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <f>params!A23</f>
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <f>params!F23</f>
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <f>params!K23</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="27">
-        <f>params!J23</f>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f>params!M23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D19" s="27"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D20" s="27"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D21" s="27"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D22" s="27"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D23" s="27"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D24" s="27"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D25" s="27"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D30" s="27"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D31" s="27"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" s="27"/>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" s="27"/>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" s="27"/>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" s="27"/>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="27"/>
     </row>
   </sheetData>
@@ -6014,54 +7537,54 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="H4" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B5">
         <f>B3/12</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L5">
         <v>2022</v>
@@ -6070,7 +7593,7 @@
         <v>64364</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B6">
         <f>B5*3</f>
         <v>5</v>
@@ -6098,7 +7621,7 @@
         <v>62700</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>2021</v>
       </c>
@@ -6120,9 +7643,9 @@
         <v>2.6539074960127591</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D8" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E8">
         <f>(E6-E7)/(E7/100)</f>
@@ -6145,7 +7668,7 @@
         <v>62700</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G9">
         <v>2019</v>
       </c>
@@ -6163,7 +7686,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G10">
         <v>2018</v>
       </c>
@@ -6183,7 +7706,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G11">
         <v>2017</v>
       </c>
@@ -6201,7 +7724,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G12">
         <v>2016</v>
       </c>
@@ -6219,7 +7742,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G13">
         <v>2015</v>
       </c>
@@ -6235,7 +7758,7 @@
         <v>127.27272727272727</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G14">
         <v>2014</v>
       </c>
@@ -6254,7 +7777,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G15">
         <v>2013</v>
       </c>
@@ -6273,10 +7796,10 @@
         <v>15714.285714285714</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G16">
         <v>2012</v>
       </c>
@@ -6287,16 +7810,16 @@
         <v>40</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="S16" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="T16" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="7:20">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="7:20" x14ac:dyDescent="0.2">
       <c r="R17">
         <v>2013</v>
       </c>
@@ -6307,7 +7830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="7:20">
+    <row r="18" spans="7:20" x14ac:dyDescent="0.2">
       <c r="H18" s="42"/>
       <c r="R18">
         <v>2014</v>
@@ -6319,7 +7842,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="7:20">
+    <row r="19" spans="7:20" x14ac:dyDescent="0.2">
       <c r="R19">
         <v>2015</v>
       </c>
@@ -6330,7 +7853,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="7:20">
+    <row r="20" spans="7:20" x14ac:dyDescent="0.2">
       <c r="R20">
         <v>2016</v>
       </c>
@@ -6341,12 +7864,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="7:20">
+    <row r="21" spans="7:20" x14ac:dyDescent="0.2">
       <c r="H21" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="R21">
         <v>2017</v>
@@ -6358,7 +7881,7 @@
         <v>191.26984126984127</v>
       </c>
     </row>
-    <row r="22" spans="7:20">
+    <row r="22" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G22">
         <v>2022</v>
       </c>
@@ -6380,7 +7903,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="7:20">
+    <row r="23" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G23">
         <v>2021</v>
       </c>
@@ -6402,7 +7925,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="24" spans="7:20">
+    <row r="24" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G24">
         <v>2020</v>
       </c>
@@ -6424,7 +7947,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="7:20">
+    <row r="25" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G25">
         <v>2019</v>
       </c>
@@ -6441,7 +7964,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="26" spans="7:20">
+    <row r="26" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G26">
         <v>2018</v>
       </c>
@@ -6458,15 +7981,15 @@
         <v>482</v>
       </c>
     </row>
-    <row r="32" spans="7:20">
+    <row r="32" spans="7:20" x14ac:dyDescent="0.2">
       <c r="H32" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="7:10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G33">
         <v>2018</v>
       </c>
@@ -6474,7 +7997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="7:10">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G34">
         <v>2019</v>
       </c>
@@ -6485,10 +8008,10 @@
         <v>40</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="7:10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G35">
         <v>2020</v>
       </c>
@@ -6499,7 +8022,7 @@
         <v>127.27272727272727</v>
       </c>
     </row>
-    <row r="36" spans="7:10">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G36">
         <v>2021</v>
       </c>
@@ -6510,7 +8033,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="37" spans="7:10">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G37">
         <v>2022</v>
       </c>
@@ -6542,9 +8065,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
@@ -6552,7 +8075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D7" s="11"/>
       <c r="E7" s="9" t="s">
         <v>10</v>
@@ -6574,7 +8097,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="s">
         <v>30</v>
       </c>
@@ -6600,7 +8123,7 @@
         <v>83.3333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
@@ -6626,7 +8149,7 @@
         <v>0.18262500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
@@ -6652,7 +8175,7 @@
         <v>18.262499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="11" t="s">
         <v>32</v>
       </c>
@@ -6678,7 +8201,7 @@
         <v>3.6525000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="11" t="s">
         <v>33</v>
       </c>
@@ -6704,7 +8227,7 @@
         <v>13.34075625</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.6">
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="I13" s="11" t="s">
         <v>33</v>
       </c>
@@ -6718,29 +8241,29 @@
         <v>3.6524999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="5:10">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="5:10">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="5:10">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="5:10">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E20" s="8"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
       <c r="J22" s="8"/>
     </row>
   </sheetData>
@@ -6757,9 +8280,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Tidy short term model excel
</commit_message>
<xml_diff>
--- a/short_term_model.xlsx
+++ b/short_term_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/eam/ICIP2023-EAM-model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Luke Benson\Documents\4th_year\Individual Project\ICIP2023-EAM-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC128D7-35E7-0840-A410-0A420A793D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78714010-9A92-413F-BEAE-0867DEB34DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="740" windowWidth="30240" windowHeight="20640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -572,11 +572,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -791,7 +791,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -820,7 +820,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -884,8 +884,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -913,7 +913,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="3" builtinId="5"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -999,7 +999,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1322,7 +1322,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1365,7 +1365,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.9377686484841572E-2"/>
+          <c:y val="0.1902314814814815"/>
+          <c:w val="0.94543942876705633"/>
+          <c:h val="0.61498432487605714"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1730,7 +1740,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2231,7 +2241,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4829,15 +4839,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>872434</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
+      <xdr:colOff>343324</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>65286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>905013</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>45278</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>5339329</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>166941</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4860,8 +4870,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17095304" y="2396435"/>
-          <a:ext cx="7277100" cy="5003800"/>
+          <a:off x="36462124" y="9067772"/>
+          <a:ext cx="6465576" cy="5098198"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4918,16 +4928,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>2012950</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4954,16 +4964,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4996,8 +5006,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2291443</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -5370,24 +5380,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.6640625" customWidth="1"/>
-    <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="59.5" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="147.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5455,7 +5478,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" s="45"/>
       <c r="B2" s="44" t="s">
         <v>17</v>
@@ -5475,7 +5498,7 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
     </row>
-    <row r="3" spans="1:22" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="100.8">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="F3" s="38">
@@ -5493,7 +5516,7 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="16.95" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>137</v>
       </c>
@@ -5527,7 +5550,7 @@
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="16.95" customHeight="1">
       <c r="B5" s="14" t="s">
         <v>159</v>
       </c>
@@ -5548,7 +5571,7 @@
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="1:22" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="28.95" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>46</v>
       </c>
@@ -5591,7 +5614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="A7" s="45"/>
       <c r="B7" s="44" t="s">
         <v>20</v>
@@ -5607,7 +5630,7 @@
       <c r="K7" s="45"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="19.95" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>45</v>
       </c>
@@ -5646,7 +5669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -5661,7 +5684,7 @@
       <c r="L9" s="32"/>
       <c r="M9" s="35"/>
     </row>
-    <row r="10" spans="1:22" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="22.95" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>44</v>
       </c>
@@ -5700,7 +5723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22">
       <c r="A11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -5710,7 +5733,7 @@
       <c r="K11" s="4"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:22" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="86.4">
       <c r="A12" s="13" t="s">
         <v>48</v>
       </c>
@@ -5744,7 +5767,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22">
       <c r="A13" s="45"/>
       <c r="B13" s="44" t="s">
         <v>24</v>
@@ -5759,7 +5782,7 @@
       <c r="J13" s="46"/>
       <c r="K13" s="45"/>
     </row>
-    <row r="14" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="24" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>124</v>
       </c>
@@ -5794,7 +5817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="F15" s="14"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -5807,14 +5830,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22">
       <c r="E16" s="13"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="34.049999999999997" customHeight="1">
       <c r="D17" s="13" t="s">
         <v>68</v>
       </c>
@@ -5831,7 +5854,7 @@
       </c>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="25.05" customHeight="1">
       <c r="D18" s="13" t="s">
         <v>67</v>
       </c>
@@ -5847,7 +5870,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="34.049999999999997" customHeight="1">
       <c r="A19" s="13" t="s">
         <v>62</v>
       </c>
@@ -5875,7 +5898,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="31.05" customHeight="1">
       <c r="A20" s="13" t="s">
         <v>126</v>
       </c>
@@ -5906,7 +5929,7 @@
       </c>
       <c r="P20" s="17"/>
     </row>
-    <row r="21" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="34.950000000000003" customHeight="1">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -5941,7 +5964,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15.6">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -5975,7 +5998,7 @@
         <v>0.46030805687203791</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="43.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -6009,7 +6032,7 @@
       </c>
       <c r="P23" s="17"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -6040,7 +6063,7 @@
         <v>65.309194809894692</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17">
       <c r="F25" s="14"/>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
@@ -6051,7 +6074,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17">
       <c r="B26" s="13"/>
       <c r="F26" s="14"/>
       <c r="G26" s="19"/>
@@ -6060,7 +6083,7 @@
       <c r="J26" s="20"/>
       <c r="P26" s="17"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17">
       <c r="A28" s="47"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
@@ -6076,7 +6099,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17">
       <c r="A29" s="13"/>
       <c r="E29" s="13" t="s">
         <v>71</v>
@@ -6096,7 +6119,7 @@
       </c>
       <c r="P29" s="17"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17">
       <c r="A30" s="13"/>
       <c r="E30" s="13" t="s">
         <v>72</v>
@@ -6115,7 +6138,7 @@
         <v>9857.4368374871538</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17">
       <c r="A31" s="13"/>
       <c r="D31">
         <v>1080</v>
@@ -6127,7 +6150,7 @@
         <v>6720.6160710000004</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17">
       <c r="E32" s="13" t="s">
         <v>73</v>
       </c>
@@ -6146,7 +6169,7 @@
       </c>
       <c r="P32" s="17"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16">
       <c r="A33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="39">
@@ -6167,7 +6190,7 @@
         <v>0.81960861056751466</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16">
       <c r="E34" s="13" t="s">
         <v>74</v>
       </c>
@@ -6179,10 +6202,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16">
       <c r="P35" s="17"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16">
       <c r="E36" s="13" t="s">
         <v>84</v>
       </c>
@@ -6194,7 +6217,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16">
       <c r="F37" s="39">
         <f>F36/1000000</f>
         <v>983974446000</v>
@@ -6203,7 +6226,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16">
       <c r="E38" s="13" t="s">
         <v>87</v>
       </c>
@@ -6216,7 +6239,7 @@
       </c>
       <c r="P38" s="17"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16">
       <c r="F39" s="39">
         <f>F38/3600000</f>
         <v>5466.5246999999999</v>
@@ -6225,10 +6248,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16">
       <c r="P41" s="17"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16">
       <c r="K47" t="s">
         <v>141</v>
       </c>
@@ -6239,7 +6262,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="10:13">
       <c r="K49" t="s">
         <v>143</v>
       </c>
@@ -6250,7 +6273,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="10:13">
       <c r="K50" t="s">
         <v>151</v>
       </c>
@@ -6261,7 +6284,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="10:13">
       <c r="J52" t="s">
         <v>145</v>
       </c>
@@ -6275,7 +6298,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="10:13">
       <c r="K53" t="s">
         <v>147</v>
       </c>
@@ -6286,7 +6309,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="10:13">
       <c r="K54" t="s">
         <v>149</v>
       </c>
@@ -6298,7 +6321,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="10:13">
       <c r="K56" t="s">
         <v>152</v>
       </c>
@@ -6310,7 +6333,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="10:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="10:13">
       <c r="L57">
         <f>L56*1000000000</f>
         <v>2.2222222222222218E-3</v>
@@ -6341,12 +6364,12 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C25"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>109</v>
       </c>
@@ -6366,7 +6389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="48" t="s">
         <v>127</v>
       </c>
@@ -6374,7 +6397,7 @@
         <v>1.4168554229999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.6">
       <c r="A3" s="48" t="s">
         <v>128</v>
       </c>
@@ -6382,7 +6405,7 @@
         <v>0.63783970300000004</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.6">
       <c r="A4" s="48" t="s">
         <v>129</v>
       </c>
@@ -6390,7 +6413,7 @@
         <v>0.37404512000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.6">
       <c r="A5" s="48" t="s">
         <v>130</v>
       </c>
@@ -6398,7 +6421,7 @@
         <v>0.31920586299999998</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.6">
       <c r="A6" s="48" t="s">
         <v>131</v>
       </c>
@@ -6406,7 +6429,7 @@
         <v>0.26436660499999998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.6">
       <c r="A7" s="48" t="s">
         <v>132</v>
       </c>
@@ -6414,7 +6437,7 @@
         <v>0.29876190600000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.6">
       <c r="A8" s="48" t="s">
         <v>133</v>
       </c>
@@ -6422,7 +6445,7 @@
         <v>0.86660710100000005</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6">
       <c r="A9" s="48" t="s">
         <v>134</v>
       </c>
@@ -6430,7 +6453,7 @@
         <v>1.514157964</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15.6">
       <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
@@ -6438,7 +6461,7 @@
         <v>1.7012569230000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="48" t="s">
         <v>136</v>
       </c>
@@ -6446,7 +6469,7 @@
         <v>1.6595511620000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15.6">
       <c r="A12" s="48" t="s">
         <v>110</v>
       </c>
@@ -6454,7 +6477,7 @@
         <v>1.5244268249999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.6">
       <c r="A13" s="48" t="s">
         <v>111</v>
       </c>
@@ -6462,7 +6485,7 @@
         <v>1.448150056</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.6">
       <c r="A14" s="48" t="s">
         <v>112</v>
       </c>
@@ -6470,7 +6493,7 @@
         <v>1.575906287</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="48" t="s">
         <v>113</v>
       </c>
@@ -6478,7 +6501,7 @@
         <v>1.7089537189999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="48" t="s">
         <v>114</v>
       </c>
@@ -6486,7 +6509,7 @@
         <v>1.593198581</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.6">
       <c r="A17" s="48" t="s">
         <v>115</v>
       </c>
@@ -6494,7 +6517,7 @@
         <v>1.802996974</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15.6">
       <c r="A18" s="48" t="s">
         <v>116</v>
       </c>
@@ -6502,7 +6525,7 @@
         <v>2.169305574</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.6">
       <c r="A19" s="48" t="s">
         <v>117</v>
       </c>
@@ -6510,7 +6533,7 @@
         <v>2.535614174</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.6">
       <c r="A20" s="48" t="s">
         <v>118</v>
       </c>
@@ -6518,7 +6541,7 @@
         <v>2.9019227750000001</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.6">
       <c r="A21" s="48" t="s">
         <v>119</v>
       </c>
@@ -6526,7 +6549,7 @@
         <v>3.188140942</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.6">
       <c r="A22" s="48" t="s">
         <v>120</v>
       </c>
@@ -6534,7 +6557,7 @@
         <v>3.4647006999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.6">
       <c r="A23" s="48" t="s">
         <v>121</v>
       </c>
@@ -6542,7 +6565,7 @@
         <v>3.4224707250000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.6">
       <c r="A24" s="48" t="s">
         <v>122</v>
       </c>
@@ -6550,7 +6573,7 @@
         <v>3.5257825880000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.6">
       <c r="A25" s="48" t="s">
         <v>123</v>
       </c>
@@ -6567,13 +6590,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6A4CB5-69F6-F447-81D4-FE2367EAF2AB}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>109</v>
       </c>
@@ -6600,7 +6636,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15.6">
       <c r="A2" s="48" t="s">
         <v>127</v>
       </c>
@@ -6613,7 +6649,7 @@
         <v>0.27255205500000002</v>
       </c>
       <c r="N2">
-        <f>M2*1000</f>
+        <f t="shared" ref="N2:N25" si="0">M2*1000</f>
         <v>272.552055</v>
       </c>
       <c r="P2" s="43">
@@ -6627,7 +6663,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.6">
       <c r="A3" s="48" t="s">
         <v>128</v>
       </c>
@@ -6648,11 +6684,11 @@
         <v>0.40799999999999997</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S25" si="0">R3*1000</f>
+        <f t="shared" ref="S3:S25" si="1">R3*1000</f>
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15.6">
       <c r="A4" s="48" t="s">
         <v>129</v>
       </c>
@@ -6663,7 +6699,7 @@
         <v>0.24877260300000001</v>
       </c>
       <c r="N4">
-        <f>M4*1000</f>
+        <f t="shared" si="0"/>
         <v>248.772603</v>
       </c>
       <c r="P4" s="43">
@@ -6673,11 +6709,11 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="S4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.6">
       <c r="A5" s="48" t="s">
         <v>130</v>
       </c>
@@ -6688,7 +6724,7 @@
         <v>0.24897123300000001</v>
       </c>
       <c r="N5">
-        <f>M5*1000</f>
+        <f t="shared" si="0"/>
         <v>248.97123300000001</v>
       </c>
       <c r="P5" s="43">
@@ -6698,11 +6734,11 @@
         <v>0.19</v>
       </c>
       <c r="S5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.6">
       <c r="A6" s="48" t="s">
         <v>131</v>
       </c>
@@ -6713,7 +6749,7 @@
         <v>0.28523698600000003</v>
       </c>
       <c r="N6">
-        <f>M6*1000</f>
+        <f t="shared" si="0"/>
         <v>285.236986</v>
       </c>
       <c r="P6" s="43">
@@ -6723,11 +6759,11 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="S6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15.6">
       <c r="A7" s="48" t="s">
         <v>132</v>
       </c>
@@ -6738,7 +6774,7 @@
         <v>0.334458904</v>
       </c>
       <c r="N7">
-        <f>M7*1000</f>
+        <f t="shared" si="0"/>
         <v>334.45890400000002</v>
       </c>
       <c r="P7" s="43">
@@ -6748,11 +6784,11 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="S7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15.6">
       <c r="A8" s="48" t="s">
         <v>133</v>
       </c>
@@ -6763,7 +6799,7 @@
         <v>0.33444383599999999</v>
       </c>
       <c r="N8">
-        <f>M8*1000</f>
+        <f t="shared" si="0"/>
         <v>334.44383599999998</v>
       </c>
       <c r="P8" s="43">
@@ -6773,11 +6809,11 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="S8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>416</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="15.6">
       <c r="A9" s="48" t="s">
         <v>134</v>
       </c>
@@ -6788,7 +6824,7 @@
         <v>0.239157534</v>
       </c>
       <c r="N9">
-        <f>M9*1000</f>
+        <f t="shared" si="0"/>
         <v>239.157534</v>
       </c>
       <c r="P9" s="43">
@@ -6798,11 +6834,11 @@
         <v>0.39500000000000002</v>
       </c>
       <c r="S9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="15.6">
       <c r="A10" s="48" t="s">
         <v>135</v>
       </c>
@@ -6813,7 +6849,7 @@
         <v>0.151635616</v>
       </c>
       <c r="N10">
-        <f>M10*1000</f>
+        <f t="shared" si="0"/>
         <v>151.635616</v>
       </c>
       <c r="P10" s="43">
@@ -6823,11 +6859,11 @@
         <v>0.224</v>
       </c>
       <c r="S10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15.6">
       <c r="A11" s="48" t="s">
         <v>136</v>
       </c>
@@ -6838,7 +6874,7 @@
         <v>0.10239588999999999</v>
       </c>
       <c r="N11">
-        <f>M11*1000</f>
+        <f t="shared" si="0"/>
         <v>102.39588999999999</v>
       </c>
       <c r="P11" s="43">
@@ -6848,11 +6884,11 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="S11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15.6">
       <c r="A12" s="48" t="s">
         <v>110</v>
       </c>
@@ -6863,7 +6899,7 @@
         <v>0.118893151</v>
       </c>
       <c r="N12">
-        <f>M12*1000</f>
+        <f t="shared" si="0"/>
         <v>118.893151</v>
       </c>
       <c r="P12" s="43">
@@ -6873,11 +6909,11 @@
         <v>0.309</v>
       </c>
       <c r="S12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15.6">
       <c r="A13" s="48" t="s">
         <v>111</v>
       </c>
@@ -6888,7 +6924,7 @@
         <v>0.148576712</v>
       </c>
       <c r="N13">
-        <f>M13*1000</f>
+        <f t="shared" si="0"/>
         <v>148.57671199999999</v>
       </c>
       <c r="P13" s="43">
@@ -6898,11 +6934,11 @@
         <v>0.253</v>
       </c>
       <c r="S13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15.6">
       <c r="A14" s="48" t="s">
         <v>112</v>
       </c>
@@ -6913,7 +6949,7 @@
         <v>0.202276712</v>
       </c>
       <c r="N14">
-        <f>M14*1000</f>
+        <f t="shared" si="0"/>
         <v>202.276712</v>
       </c>
       <c r="P14" s="43">
@@ -6923,11 +6959,11 @@
         <v>0.28100000000000003</v>
       </c>
       <c r="S14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15.6">
       <c r="A15" s="48" t="s">
         <v>113</v>
       </c>
@@ -6938,7 +6974,7 @@
         <v>0.15460137000000002</v>
       </c>
       <c r="N15">
-        <f>M15*1000</f>
+        <f t="shared" si="0"/>
         <v>154.60137</v>
       </c>
       <c r="P15" s="43">
@@ -6948,11 +6984,11 @@
         <v>0.188</v>
       </c>
       <c r="S15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15.6">
       <c r="A16" s="48" t="s">
         <v>114</v>
       </c>
@@ -6963,7 +6999,7 @@
         <v>0.124071233</v>
       </c>
       <c r="N16">
-        <f>M16*1000</f>
+        <f t="shared" si="0"/>
         <v>124.07123300000001</v>
       </c>
       <c r="P16" s="43">
@@ -6973,11 +7009,11 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="S16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="15.6">
       <c r="A17" s="48" t="s">
         <v>115</v>
       </c>
@@ -6988,7 +7024,7 @@
         <v>0.208646575</v>
       </c>
       <c r="N17">
-        <f>M17*1000</f>
+        <f t="shared" si="0"/>
         <v>208.64657500000001</v>
       </c>
       <c r="P17" s="43">
@@ -6998,11 +7034,11 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="S17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="15.6">
       <c r="A18" s="48" t="s">
         <v>116</v>
       </c>
@@ -7013,7 +7049,7 @@
         <v>0.177216438</v>
       </c>
       <c r="N18">
-        <f>M18*1000</f>
+        <f t="shared" si="0"/>
         <v>177.21643800000001</v>
       </c>
       <c r="P18" s="43">
@@ -7023,11 +7059,11 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="S18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>417</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="15.6">
       <c r="A19" s="48" t="s">
         <v>117</v>
       </c>
@@ -7038,7 +7074,7 @@
         <v>0.121783562</v>
       </c>
       <c r="N19">
-        <f>M19*1000</f>
+        <f t="shared" si="0"/>
         <v>121.783562</v>
       </c>
       <c r="P19" s="43">
@@ -7048,11 +7084,11 @@
         <v>0.25800000000000001</v>
       </c>
       <c r="S19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="15.6">
       <c r="A20" s="48" t="s">
         <v>118</v>
       </c>
@@ -7063,7 +7099,7 @@
         <v>0.147079452</v>
       </c>
       <c r="N20">
-        <f>M20*1000</f>
+        <f t="shared" si="0"/>
         <v>147.079452</v>
       </c>
       <c r="P20" s="43">
@@ -7073,11 +7109,11 @@
         <v>0.245</v>
       </c>
       <c r="S20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="15.6">
       <c r="A21" s="48" t="s">
         <v>119</v>
       </c>
@@ -7088,7 +7124,7 @@
         <v>0.175157534</v>
       </c>
       <c r="N21">
-        <f>M21*1000</f>
+        <f t="shared" si="0"/>
         <v>175.157534</v>
       </c>
       <c r="P21" s="43">
@@ -7098,11 +7134,11 @@
         <v>0.248</v>
       </c>
       <c r="S21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="15.6">
       <c r="A22" s="48" t="s">
         <v>120</v>
       </c>
@@ -7113,7 +7149,7 @@
         <v>0.29710000000000003</v>
       </c>
       <c r="N22">
-        <f>M22*1000</f>
+        <f t="shared" si="0"/>
         <v>297.10000000000002</v>
       </c>
       <c r="P22" s="43">
@@ -7123,11 +7159,11 @@
         <v>0.34</v>
       </c>
       <c r="S22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>340</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="15.6">
       <c r="A23" s="48" t="s">
         <v>121</v>
       </c>
@@ -7138,7 +7174,7 @@
         <v>0.37654520499999999</v>
       </c>
       <c r="N23">
-        <f>M23*1000</f>
+        <f t="shared" si="0"/>
         <v>376.54520500000001</v>
       </c>
       <c r="P23" s="43">
@@ -7148,11 +7184,11 @@
         <v>0.50700000000000001</v>
       </c>
       <c r="S23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>507</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="15.6">
       <c r="A24" s="48" t="s">
         <v>122</v>
       </c>
@@ -7163,7 +7199,7 @@
         <v>0.38226712300000004</v>
       </c>
       <c r="N24">
-        <f>M24*1000</f>
+        <f t="shared" si="0"/>
         <v>382.26712300000003</v>
       </c>
       <c r="P24" s="43">
@@ -7173,11 +7209,11 @@
         <v>0.35899999999999999</v>
       </c>
       <c r="S24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>359</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="15.6">
       <c r="A25" s="48" t="s">
         <v>123</v>
       </c>
@@ -7188,7 +7224,7 @@
         <v>0.36048767099999995</v>
       </c>
       <c r="N25">
-        <f>M25*1000</f>
+        <f t="shared" si="0"/>
         <v>360.48767099999998</v>
       </c>
       <c r="P25" s="43">
@@ -7198,11 +7234,11 @@
         <v>0.32600000000000001</v>
       </c>
       <c r="S25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="15.6">
       <c r="A26" s="43"/>
     </row>
   </sheetData>
@@ -7215,13 +7251,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAF771D-6F80-F045-B144-615B3F88F36B}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="A1:F17"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="252.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>161</v>
       </c>
@@ -7241,10 +7285,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="str">
         <f>params!A6</f>
         <v>I_Tx</v>
@@ -7266,10 +7310,10 @@
         <v>OpenConnect Appliances. https://openconnect.netflix.com/en_gb/appliances/ - lists ideal energy intensity values during full utilisation. From the list of appliances we calculate the marginal energy intensity, assuming 40% base power and PUE of 1.5. Cautiously select the least energy efficient one (9J/Gb).</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="D4" s="27"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="str">
         <f>params!A8</f>
         <v>I_Core</v>
@@ -7291,10 +7335,10 @@
         <v>The power consumption of mobile and fixed network data services - The case of streaming video and downloading large files</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="D6" s="27"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="str">
         <f>params!A10</f>
         <v>I_Acc</v>
@@ -7316,10 +7360,10 @@
         <v>The power consumption of mobile and fixed network data services - The case of streaming video and downloading large files</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="D8" s="27"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="str">
         <f>params!A12</f>
         <v>cachemiss_rate</v>
@@ -7341,10 +7385,10 @@
         <v>https://support.google.com/interconnect/answer/9058809?hl=en</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="D10" s="27"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="str">
         <f>params!A14</f>
         <v>carbon_intensity</v>
@@ -7366,13 +7410,13 @@
         <v>Combined Cycle Gas. -https://github.com/carbon-intensity/methodology/raw/master/Carbon%20Intensity%20Forecast%20Methodology.pdf</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="D12" s="27"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="str">
         <f>params!A19</f>
         <v>daily_audience</v>
@@ -7395,7 +7439,7 @@
 Ofcom finds the viewing time has remained largely similar since pandemic (https://www.ofcom.org.uk/__data/assets/pdf_file/0016/242701/media-nations-report-2022.pdf)</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="str">
         <f>params!A20</f>
         <v>viewing_time</v>
@@ -7417,7 +7461,7 @@
         <v>https://www.ofcom.org.uk/__data/assets/pdf_file/0016/242701/media-nations-report-2022.pdf</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="str">
         <f>params!A21</f>
         <v>bitrate</v>
@@ -7439,7 +7483,7 @@
         <v>Own</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="str">
         <f>params!A23</f>
         <v>power_decoding</v>
@@ -7461,67 +7505,67 @@
         <v>Own measurements</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="D18" s="27"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="D19" s="27"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="D20" s="27"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="D21" s="27"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="D22" s="27"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="D23" s="27"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="D24" s="27"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="D25" s="27"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="D30" s="27"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="D31" s="27"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:4">
       <c r="D33" s="27"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:4">
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:4">
       <c r="D35" s="27"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:4">
       <c r="D36" s="27"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:4">
       <c r="D37" s="27"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:4">
       <c r="D38" s="27"/>
     </row>
   </sheetData>
@@ -7533,21 +7577,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004DC5D5-94B1-FE4A-8A6C-ACB9A57C077A}">
   <dimension ref="A2:T37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="34.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="A3" s="13" t="s">
         <v>90</v>
       </c>
@@ -7558,7 +7616,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="13" t="s">
         <v>91</v>
       </c>
@@ -7572,7 +7630,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="A5" s="13" t="s">
         <v>92</v>
       </c>
@@ -7593,7 +7651,7 @@
         <v>64364</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="B6">
         <f>B5*3</f>
         <v>5</v>
@@ -7621,7 +7679,7 @@
         <v>62700</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="D7">
         <v>2021</v>
       </c>
@@ -7643,7 +7701,7 @@
         <v>2.6539074960127591</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="D8" s="13" t="s">
         <v>93</v>
       </c>
@@ -7668,7 +7726,7 @@
         <v>62700</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="G9">
         <v>2019</v>
       </c>
@@ -7686,7 +7744,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="G10">
         <v>2018</v>
       </c>
@@ -7706,7 +7764,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20">
       <c r="G11">
         <v>2017</v>
       </c>
@@ -7724,7 +7782,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="G12">
         <v>2016</v>
       </c>
@@ -7742,7 +7800,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20">
       <c r="G13">
         <v>2015</v>
       </c>
@@ -7758,7 +7816,7 @@
         <v>127.27272727272727</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="G14">
         <v>2014</v>
       </c>
@@ -7777,7 +7835,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="G15">
         <v>2013</v>
       </c>
@@ -7799,7 +7857,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="G16">
         <v>2012</v>
       </c>
@@ -7819,7 +7877,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:20">
       <c r="R17">
         <v>2013</v>
       </c>
@@ -7830,7 +7888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:20">
       <c r="H18" s="42"/>
       <c r="R18">
         <v>2014</v>
@@ -7842,7 +7900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:20">
       <c r="R19">
         <v>2015</v>
       </c>
@@ -7853,7 +7911,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:20">
       <c r="R20">
         <v>2016</v>
       </c>
@@ -7864,7 +7922,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:20">
       <c r="H21" s="13" t="s">
         <v>100</v>
       </c>
@@ -7881,7 +7939,7 @@
         <v>191.26984126984127</v>
       </c>
     </row>
-    <row r="22" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:20">
       <c r="G22">
         <v>2022</v>
       </c>
@@ -7903,7 +7961,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:20">
       <c r="G23">
         <v>2021</v>
       </c>
@@ -7925,7 +7983,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="24" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:20">
       <c r="G24">
         <v>2020</v>
       </c>
@@ -7947,7 +8005,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="7:20">
       <c r="G25">
         <v>2019</v>
       </c>
@@ -7964,7 +8022,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="26" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="7:20">
       <c r="G26">
         <v>2018</v>
       </c>
@@ -7981,7 +8039,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="32" spans="7:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="7:20">
       <c r="H32" s="13" t="s">
         <v>107</v>
       </c>
@@ -7989,7 +8047,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10">
       <c r="G33">
         <v>2018</v>
       </c>
@@ -7997,7 +8055,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10">
       <c r="G34">
         <v>2019</v>
       </c>
@@ -8011,7 +8069,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10">
       <c r="G35">
         <v>2020</v>
       </c>
@@ -8022,7 +8080,7 @@
         <v>127.27272727272727</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10">
       <c r="G36">
         <v>2021</v>
       </c>
@@ -8033,7 +8091,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10">
       <c r="G37">
         <v>2022</v>
       </c>
@@ -8062,12 +8120,12 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
@@ -8075,7 +8133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="D7" s="11"/>
       <c r="E7" s="9" t="s">
         <v>10</v>
@@ -8097,7 +8155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="D8" s="11" t="s">
         <v>30</v>
       </c>
@@ -8123,7 +8181,7 @@
         <v>83.3333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
@@ -8149,7 +8207,7 @@
         <v>0.18262500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
@@ -8175,7 +8233,7 @@
         <v>18.262499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="D11" s="11" t="s">
         <v>32</v>
       </c>
@@ -8201,7 +8259,7 @@
         <v>3.6525000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="D12" s="11" t="s">
         <v>33</v>
       </c>
@@ -8227,7 +8285,7 @@
         <v>13.34075625</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="I13" s="11" t="s">
         <v>33</v>
       </c>
@@ -8241,29 +8299,29 @@
         <v>3.6524999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:10">
       <c r="E17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:10">
       <c r="E18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:10">
       <c r="E19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:10">
       <c r="E20" s="8"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:10">
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:10">
       <c r="J22" s="8"/>
     </row>
   </sheetData>
@@ -8280,9 +8338,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>39</v>
       </c>

</xml_diff>